<commit_message>
feat: re-export data model as lds shp format
</commit_message>
<xml_diff>
--- a/packages/data/topo50-import/model/export/lds/lds_field_mapping.xlsx
+++ b/packages/data/topo50-import/model/export/lds/lds_field_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B94AD4-3EFE-4132-926D-0035EB413217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E1128B-F895-4FF9-8FF7-02F0F9121CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32340" yWindow="3075" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="243">
   <si>
     <t>filename</t>
   </si>
@@ -454,24 +454,9 @@
     <t>road_cl</t>
   </si>
   <si>
-    <t>lol_sufi</t>
-  </si>
-  <si>
-    <t>road_access</t>
-  </si>
-  <si>
-    <t>width</t>
-  </si>
-  <si>
-    <t>name_id</t>
-  </si>
-  <si>
     <t>surface</t>
   </si>
   <si>
-    <t>num_lanes</t>
-  </si>
-  <si>
     <t>hway_num</t>
   </si>
   <si>
@@ -730,37 +715,40 @@
     <t>lane_count</t>
   </si>
   <si>
+    <t>structure_type</t>
+  </si>
+  <si>
+    <t>stored_item</t>
+  </si>
+  <si>
+    <t>tunnel_use</t>
+  </si>
+  <si>
+    <t>tunnel_use2</t>
+  </si>
+  <si>
+    <t>structure_use</t>
+  </si>
+  <si>
+    <t>info_display</t>
+  </si>
+  <si>
+    <t>place_type</t>
+  </si>
+  <si>
+    <t>temperature_indicator</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>tunnel_type</t>
+  </si>
+  <si>
+    <t>rna_sufi</t>
+  </si>
+  <si>
     <t>highway_number</t>
-  </si>
-  <si>
-    <t>structure_type</t>
-  </si>
-  <si>
-    <t>stored_item</t>
-  </si>
-  <si>
-    <t>tunnel_use</t>
-  </si>
-  <si>
-    <t>tunnel_use2</t>
-  </si>
-  <si>
-    <t>structure_use</t>
-  </si>
-  <si>
-    <t>info_display</t>
-  </si>
-  <si>
-    <t>place_type</t>
-  </si>
-  <si>
-    <t>temperature_indicator</t>
-  </si>
-  <si>
-    <t>designation</t>
-  </si>
-  <si>
-    <t>tunnel_type</t>
   </si>
 </sst>
 </file>
@@ -1132,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D597"/>
+  <dimension ref="A1:D596"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
-      <selection activeCell="C501" sqref="C501"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="A280" sqref="A280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1268,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -1350,7 +1338,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1392,7 +1380,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1602,7 +1590,7 @@
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -1630,7 +1618,7 @@
         <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D35">
         <v>4</v>
@@ -1644,7 +1632,7 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D36">
         <v>5</v>
@@ -1714,7 +1702,7 @@
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1756,7 +1744,7 @@
         <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D44">
         <v>4</v>
@@ -1854,7 +1842,7 @@
         <v>25</v>
       </c>
       <c r="C51" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D51">
         <v>3</v>
@@ -1966,7 +1954,7 @@
         <v>29</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -2008,7 +1996,7 @@
         <v>31</v>
       </c>
       <c r="C62" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -2190,7 +2178,7 @@
         <v>35</v>
       </c>
       <c r="C75" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -2526,7 +2514,7 @@
         <v>44</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D99">
         <v>3</v>
@@ -2540,7 +2528,7 @@
         <v>45</v>
       </c>
       <c r="C100" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D100">
         <v>4</v>
@@ -2708,7 +2696,7 @@
         <v>50</v>
       </c>
       <c r="C112" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D112">
         <v>2</v>
@@ -2904,7 +2892,7 @@
         <v>13</v>
       </c>
       <c r="C126" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D126">
         <v>2</v>
@@ -2946,7 +2934,7 @@
         <v>57</v>
       </c>
       <c r="C129" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D129">
         <v>2</v>
@@ -3156,7 +3144,7 @@
         <v>13</v>
       </c>
       <c r="C144" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D144">
         <v>2</v>
@@ -3226,7 +3214,7 @@
         <v>15</v>
       </c>
       <c r="C149" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D149">
         <v>1</v>
@@ -3422,7 +3410,7 @@
         <v>15</v>
       </c>
       <c r="C163" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D163">
         <v>1</v>
@@ -3450,7 +3438,7 @@
         <v>31</v>
       </c>
       <c r="C165" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D165">
         <v>3</v>
@@ -3898,7 +3886,7 @@
         <v>80</v>
       </c>
       <c r="C197" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D197">
         <v>2</v>
@@ -3996,7 +3984,7 @@
         <v>84</v>
       </c>
       <c r="C204" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D204">
         <v>3</v>
@@ -4108,7 +4096,7 @@
         <v>16</v>
       </c>
       <c r="C212" t="s">
-        <v>16</v>
+        <v>187</v>
       </c>
       <c r="D212">
         <v>2</v>
@@ -4150,7 +4138,7 @@
         <v>16</v>
       </c>
       <c r="C215" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D215">
         <v>2</v>
@@ -4304,7 +4292,7 @@
         <v>84</v>
       </c>
       <c r="C226" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D226">
         <v>4</v>
@@ -4332,7 +4320,7 @@
         <v>91</v>
       </c>
       <c r="C228" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D228">
         <v>6</v>
@@ -4346,7 +4334,7 @@
         <v>92</v>
       </c>
       <c r="C229" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D229">
         <v>7</v>
@@ -4696,7 +4684,7 @@
         <v>101</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D254">
         <v>4</v>
@@ -4808,7 +4796,7 @@
         <v>101</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D262">
         <v>4</v>
@@ -5256,7 +5244,7 @@
         <v>116</v>
       </c>
       <c r="C294" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D294">
         <v>2</v>
@@ -5354,7 +5342,7 @@
         <v>118</v>
       </c>
       <c r="C301" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D301">
         <v>5</v>
@@ -5396,7 +5384,7 @@
         <v>120</v>
       </c>
       <c r="C304" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D304">
         <v>2</v>
@@ -5452,7 +5440,7 @@
         <v>15</v>
       </c>
       <c r="C308" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D308">
         <v>1</v>
@@ -5648,7 +5636,7 @@
         <v>125</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D322">
         <v>5</v>
@@ -5662,7 +5650,7 @@
         <v>126</v>
       </c>
       <c r="C323" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D323">
         <v>6</v>
@@ -5746,7 +5734,7 @@
         <v>125</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D329">
         <v>5</v>
@@ -5760,7 +5748,7 @@
         <v>126</v>
       </c>
       <c r="C330" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D330">
         <v>6</v>
@@ -5970,7 +5958,7 @@
         <v>130</v>
       </c>
       <c r="C345" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D345">
         <v>7</v>
@@ -5984,7 +5972,7 @@
         <v>131</v>
       </c>
       <c r="C346" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D346">
         <v>8</v>
@@ -6292,7 +6280,7 @@
         <v>35</v>
       </c>
       <c r="C368" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D368">
         <v>5</v>
@@ -6527,10 +6515,10 @@
         <v>143</v>
       </c>
       <c r="B385" t="s">
-        <v>144</v>
+        <v>6</v>
       </c>
       <c r="C385" t="s">
-        <v>144</v>
+        <v>6</v>
       </c>
       <c r="D385">
         <v>2</v>
@@ -6541,10 +6529,10 @@
         <v>143</v>
       </c>
       <c r="B386" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C386" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D386">
         <v>3</v>
@@ -6555,13 +6543,13 @@
         <v>143</v>
       </c>
       <c r="B387" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="C387" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="D387">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
@@ -6569,13 +6557,13 @@
         <v>143</v>
       </c>
       <c r="B388" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C388" t="s">
-        <v>146</v>
+        <v>242</v>
       </c>
       <c r="D388">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
@@ -6583,13 +6571,13 @@
         <v>143</v>
       </c>
       <c r="B389" t="s">
-        <v>147</v>
+        <v>241</v>
       </c>
       <c r="C389" t="s">
-        <v>147</v>
+        <v>241</v>
       </c>
       <c r="D389">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
@@ -6597,13 +6585,13 @@
         <v>143</v>
       </c>
       <c r="B390" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
       <c r="C390" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
       <c r="D390">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
@@ -6611,13 +6599,13 @@
         <v>143</v>
       </c>
       <c r="B391" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="C391" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="D391">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
@@ -6625,13 +6613,13 @@
         <v>143</v>
       </c>
       <c r="B392" t="s">
-        <v>149</v>
+        <v>12</v>
       </c>
       <c r="C392" t="s">
-        <v>235</v>
+        <v>12</v>
       </c>
       <c r="D392">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
@@ -6639,13 +6627,13 @@
         <v>143</v>
       </c>
       <c r="B393" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C393" t="s">
-        <v>236</v>
+        <v>144</v>
       </c>
       <c r="D393">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
@@ -6653,2085 +6641,2085 @@
         <v>143</v>
       </c>
       <c r="B394" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
       <c r="C394" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
       <c r="D394">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B395" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C395" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="D395">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B396" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C396" t="s">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="D396">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B397" t="s">
-        <v>5</v>
+        <v>148</v>
       </c>
       <c r="C397" t="s">
-        <v>5</v>
+        <v>148</v>
       </c>
       <c r="D397">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B398" t="s">
-        <v>153</v>
+        <v>41</v>
       </c>
       <c r="C398" t="s">
-        <v>153</v>
+        <v>41</v>
       </c>
       <c r="D398">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B399" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C399" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D399">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B400" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C400" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D400">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B401" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C401" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D401">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B402" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C402" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D402">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B403" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C403" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D403">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B404" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C404" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D404">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B405" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C405" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D405">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B406" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C406" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D406">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B407" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C407" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D407">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B408" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C408" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D408">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B409" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C409" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D409">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B410" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C410" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D410">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B411" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C411" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D411">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B412" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C412" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D412">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B413" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C413" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D413">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B414" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C414" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D414">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B415" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="C415" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="D415">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B416" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C416" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D416">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B417" t="s">
-        <v>157</v>
+        <v>9</v>
       </c>
       <c r="C417" t="s">
-        <v>157</v>
+        <v>9</v>
       </c>
       <c r="D417">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B418" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C418" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="D418">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B419" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C419" t="s">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="D419">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B420" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="C420" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D420">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B421" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C421" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D421">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B422" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C422" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D422">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B423" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C423" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D423">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B424" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C424" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D424">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B425" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C425" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D425">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B426" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C426" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D426">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B427" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C427" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D427">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B428" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C428" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D428">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B429" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C429" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D429">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B430" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C430" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D430">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B431" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C431" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D431">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B432" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C432" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D432">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B433" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C433" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D433">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B434" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C434" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D434">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B435" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C435" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D435">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B436" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="C436" t="s">
-        <v>5</v>
+        <v>235</v>
       </c>
       <c r="D436">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B437" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
       <c r="C437" t="s">
-        <v>241</v>
+        <v>9</v>
       </c>
       <c r="D437">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B438" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C438" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D438">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B439" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C439" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D439">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B440" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C440" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D440">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B441" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C441" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D441">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B442" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C442" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D442">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B443" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C443" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D443">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B444" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C444" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D444">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B445" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C445" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D445">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B446" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C446" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D446">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B447" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C447" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D447">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B448" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C448" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D448">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B449" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C449" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D449">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B450" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C450" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D450">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B451" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C451" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D451">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B452" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C452" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D452">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B453" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C453" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D453">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B454" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C454" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D454">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B455" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C455" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D455">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B456" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C456" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D456">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B457" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C457" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D457">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B458" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C458" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D458">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B459" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C459" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D459">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B460" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C460" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D460">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B461" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C461" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D461">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B462" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C462" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D462">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B463" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C463" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D463">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B464" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C464" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D464">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B465" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C465" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D465">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B466" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C466" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D466">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B467" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C467" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D467">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B468" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C468" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D468">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B469" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C469" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D469">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B470" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C470" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="D470">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B471" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C471" t="s">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="D471">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B472" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C472" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D472">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B473" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C473" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D473">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B474" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C474" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D474">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B475" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C475" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D475">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B476" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C476" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D476">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B477" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C477" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D477">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B478" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C478" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D478">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B479" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C479" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D479">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B480" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C480" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D480">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B481" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C481" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D481">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B482" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C482" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D482">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B483" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C483" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D483">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B484" t="s">
-        <v>8</v>
-      </c>
-      <c r="C484" t="s">
-        <v>8</v>
+        <v>177</v>
+      </c>
+      <c r="C484" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="D484">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B485" t="s">
-        <v>182</v>
-      </c>
-      <c r="C485" s="2" t="s">
-        <v>244</v>
+        <v>9</v>
+      </c>
+      <c r="C485" t="s">
+        <v>9</v>
       </c>
       <c r="D485">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B486" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C486" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D486">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B487" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C487" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D487">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B488" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C488" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D488">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B489" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C489" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D489">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B490" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C490" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D490">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B491" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C491" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D491">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B492" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C492" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D492">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B493" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C493" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D493">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B494" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C494" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D494">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B495" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C495" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D495">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B496" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C496" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D496">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B497" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C497" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D497">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B498" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C498" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D498">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B499" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="C499" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="D499">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B500" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C500" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D500">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B501" t="s">
-        <v>188</v>
+        <v>9</v>
       </c>
       <c r="C501" t="s">
-        <v>237</v>
+        <v>9</v>
       </c>
       <c r="D501">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B502" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C502" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D502">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B503" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="C503" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="D503">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B504" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C504" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D504">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B505" t="s">
-        <v>188</v>
+        <v>9</v>
       </c>
       <c r="C505" t="s">
-        <v>237</v>
+        <v>9</v>
       </c>
       <c r="D505">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B506" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C506" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D506">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B507" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C507" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D507">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B508" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C508" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D508">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B509" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
       <c r="C509" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
       <c r="D509">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B510" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="C510" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="D510">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B511" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C511" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D511">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B512" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C512" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D512">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B513" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C513" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D513">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B514" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C514" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D514">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B515" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C515" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D515">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B516" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="C516" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="D516">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B517" t="s">
-        <v>125</v>
-      </c>
-      <c r="C517" s="2" t="s">
-        <v>231</v>
+        <v>126</v>
+      </c>
+      <c r="C517" t="s">
+        <v>126</v>
       </c>
       <c r="D517">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B518" t="s">
-        <v>126</v>
-      </c>
-      <c r="C518" s="2" t="s">
-        <v>232</v>
+        <v>9</v>
+      </c>
+      <c r="C518" t="s">
+        <v>9</v>
       </c>
       <c r="D518">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B519" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C519" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D519">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B520" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C520" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D520">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B521" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C521" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D521">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B522" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C522" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D522">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B523" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C523" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D523">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B524" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C524" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D524">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B525" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="C525" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D525">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B526" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C526" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D526">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B527" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C527" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D527">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B528" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C528" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D528">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B529" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C529" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D529">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B530" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C530" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D530">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B531" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C531" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D531">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B532" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C532" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D532">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B533" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C533" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D533">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B534" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C534" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D534">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B535" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C535" t="s">
-        <v>12</v>
+        <v>240</v>
       </c>
       <c r="D535">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B536" t="s">
-        <v>13</v>
+        <v>192</v>
       </c>
       <c r="C536" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="D536">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B537" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C537" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D537">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B538" t="s">
-        <v>198</v>
+        <v>9</v>
       </c>
       <c r="C538" t="s">
-        <v>240</v>
+        <v>9</v>
       </c>
       <c r="D538">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B539" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C539" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D539">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B540" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C540" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D540">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B541" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C541" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D541">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B542" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C542" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D542">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.25">
@@ -8739,776 +8727,762 @@
         <v>200</v>
       </c>
       <c r="B543" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C543" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D543">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B544" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C544" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D544">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B545" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C545" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D545">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B546" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C546" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D546">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B547" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C547" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D547">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B548" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C548" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D548">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B549" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C549" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D549">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B550" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C550" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D550">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B551" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C551" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D551">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B552" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C552" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D552">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B553" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="C553" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="D553">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="554" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B554" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="C554" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D554">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="555" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B555" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C555" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D555">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B556" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C556" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D556">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="557" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B557" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C557" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D557">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B558" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C558" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D558">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B559" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="C559" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="D559">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B560" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="C560" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D560">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B561" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C561" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="D561">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B562" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C562" t="s">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="D562">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B563" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C563" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D563">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B564" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C564" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D564">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B565" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C565" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D565">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B566" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="C566" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="D566">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="567" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B567" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="C567" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D567">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="568" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B568" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C568" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D568">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B569" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C569" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D569">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B570" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C570" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D570">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B571" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C571" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D571">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="572" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B572" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="C572" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="D572">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="573" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B573" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="C573" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D573">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="574" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B574" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C574" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D574">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="575" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B575" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C575" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D575">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="576" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B576" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C576" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D576">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="577" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B577" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C577" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D577">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="578" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B578" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C578" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D578">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="579" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B579" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C579" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D579">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B580" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C580" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D580">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B581" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C581" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D581">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="582" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B582" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C582" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D582">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="583" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B583" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C583" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D583">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="584" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B584" t="s">
-        <v>12</v>
+        <v>204</v>
       </c>
       <c r="C584" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="D584">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B585" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C585" t="s">
-        <v>241</v>
+        <v>9</v>
       </c>
       <c r="D585">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B586" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C586" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D586">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B587" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C587" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D587">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B588" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C588" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D588">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="589" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B589" t="s">
-        <v>5</v>
+        <v>207</v>
       </c>
       <c r="C589" t="s">
-        <v>5</v>
+        <v>235</v>
       </c>
       <c r="D589">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="590" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B590" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="C590" t="s">
-        <v>241</v>
+        <v>9</v>
       </c>
       <c r="D590">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="591" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B591" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C591" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D591">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="592" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B592" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C592" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D592">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="593" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B593" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C593" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D593">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="594" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B594" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C594" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D594">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="595" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B595" t="s">
-        <v>8</v>
+        <v>209</v>
       </c>
       <c r="C595" t="s">
-        <v>8</v>
+        <v>209</v>
       </c>
       <c r="D595">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B596" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="C596" t="s">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="D596">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="597" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A597" t="s">
-        <v>213</v>
-      </c>
-      <c r="B597" t="s">
-        <v>9</v>
-      </c>
-      <c r="C597" t="s">
-        <v>9</v>
-      </c>
-      <c r="D597">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D600">
-    <sortCondition ref="A2:A600"/>
-    <sortCondition ref="D2:D600"/>
-    <sortCondition ref="B2:B600"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D599">
+    <sortCondition ref="A2:A599"/>
+    <sortCondition ref="D2:D599"/>
+    <sortCondition ref="B2:B599"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>